<commit_message>
added images, did some styling
</commit_message>
<xml_diff>
--- a/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
+++ b/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
@@ -422,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -439,6 +439,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -637,7 +640,7 @@
       <c r="AD1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="2">
@@ -674,7 +677,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2">
@@ -724,7 +727,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="2">
@@ -765,7 +768,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="2">
@@ -821,7 +824,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B6" s="2">
@@ -870,7 +873,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="2">
@@ -929,7 +932,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B8" s="2">
@@ -964,7 +967,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="2">
@@ -1001,7 +1004,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="2">
@@ -1035,7 +1038,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="2">
@@ -1069,7 +1072,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="2">
@@ -1103,7 +1106,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B13" s="2">
@@ -1137,7 +1140,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B14" s="2">
@@ -1171,7 +1174,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B15" s="2">
@@ -1205,7 +1208,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B16" s="2">
@@ -1216,7 +1219,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B17" s="2">
@@ -1245,7 +1248,7 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2">
@@ -1268,7 +1271,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B20" s="2">
@@ -1312,7 +1315,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B24" s="2">
@@ -1334,7 +1337,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="6" t="s">
         <v>79</v>
       </c>
       <c r="B26" s="2">
@@ -1345,7 +1348,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B27" s="2">
@@ -1356,7 +1359,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B28" s="2">
@@ -1381,7 +1384,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="2">
@@ -1403,7 +1406,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B31" s="2">
@@ -1414,7 +1417,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="6" t="s">
         <v>86</v>
       </c>
       <c r="B32" s="2">
@@ -1425,7 +1428,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B33" s="2">
@@ -1436,7 +1439,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B34" s="2">
@@ -1447,7 +1450,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B35" s="2">
@@ -1469,7 +1472,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="6" t="s">
         <v>92</v>
       </c>
       <c r="B37" s="2">
@@ -1480,7 +1483,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="6" t="s">
         <v>93</v>
       </c>
       <c r="B38" s="2">
@@ -1491,7 +1494,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="6" t="s">
         <v>94</v>
       </c>
       <c r="B39" s="2">
@@ -1502,7 +1505,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B40" s="2">
@@ -1524,7 +1527,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="6" t="s">
         <v>98</v>
       </c>
       <c r="B42" s="2">
@@ -1535,7 +1538,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B43" s="2">
@@ -1546,7 +1549,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="6" t="s">
         <v>100</v>
       </c>
       <c r="B44" s="2">
@@ -1562,7 +1565,7 @@
       <c r="U44" s="2"/>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B45" s="2">
@@ -1577,7 +1580,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B46" s="2">
@@ -1588,7 +1591,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B47" s="2">
@@ -1599,7 +1602,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B48" s="2">
@@ -1626,7 +1629,7 @@
       <c r="U48" s="2"/>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B49" s="2">
@@ -1637,7 +1640,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B50" s="2">
@@ -1648,7 +1651,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="6" t="s">
         <v>107</v>
       </c>
       <c r="B51" s="2">
@@ -1659,7 +1662,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B52" s="2">
@@ -1687,7 +1690,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B53" s="2">
@@ -1706,7 +1709,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B54" s="2">
@@ -1717,7 +1720,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B55" s="2">
@@ -1728,7 +1731,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B56" s="2">
@@ -1739,7 +1742,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B57" s="2">
@@ -1750,7 +1753,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B58" s="2">
@@ -1779,10 +1782,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the filters for mobile
</commit_message>
<xml_diff>
--- a/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
+++ b/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="421">
   <si>
     <t>name</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>The best film of 2015 must, alas, join the long list of deserving projects that were overlooked by the Oscars' Best Picture category. (At least it's in good company.) Blanchett and Mara play two women navigating a love affair in 1950s New York, even though neither is quite willing to label it as such. This is a tremendous movie about feeling all alone in the world, then finding somebody else to feel a little bit less alone with, and in its beautiful images and marvelous performances it courses with deeply buried emotions. Oscar didn't recognize &lt;i&gt;Carol &lt;/i&gt;for its top prize; history surely will.</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://www.vox.com/culture/2015/11/20/9769890/carol-movie-review"&gt;Read our review&lt;/a&gt;.</t>
   </si>
   <si>
     <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/679wr31SXWk" frameborder="0" allowfullscreen&gt;&lt;/iframe&gt;</t>
@@ -1519,1720 +1522,1723 @@
       <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2">
         <v>2.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2">
         <v>3.0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2">
         <v>4.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2">
         <v>5.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2">
         <v>6.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C8" s="2">
         <v>7.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2">
         <v>8.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2">
         <v>9.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2">
         <v>10.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C12" s="2">
         <v>11.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C13" s="2">
         <v>12.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C14" s="2">
         <v>13.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C15" s="2">
         <v>14.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C16" s="2">
         <v>15.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C17" s="2">
         <v>16.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C18" s="2">
         <v>17.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C19" s="2">
         <v>18.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C20" s="2">
         <v>19.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C21" s="2">
         <v>20.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C22" s="2">
         <v>21.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C23" s="2">
         <v>22.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C24" s="2">
         <v>23.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C25" s="2">
         <v>24.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C26" s="2">
         <v>25.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C27" s="2">
         <v>26.0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C28" s="2">
         <v>27.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C29" s="2">
         <v>28.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C30" s="2">
         <v>29.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C31" s="2">
         <v>30.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C32" s="2">
         <v>31.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C33" s="2">
         <v>32.0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C34" s="2">
         <v>33.0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C35" s="2">
         <v>34.0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C36" s="2">
         <v>35.0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C37" s="2">
         <v>36.0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C38" s="2">
         <v>37.0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C39" s="2">
         <v>38.0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C40" s="2">
         <v>39.0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C41" s="2">
         <v>40.0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C42" s="2">
         <v>41.0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C43" s="2">
         <v>42.0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C44" s="2">
         <v>43.0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C45" s="2">
         <v>44.0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C46" s="2">
         <v>45.0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C47" s="2">
         <v>46.0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C48" s="2">
         <v>47.0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C49" s="2">
         <v>48.0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C50" s="2">
         <v>49.0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C51" s="2">
         <v>50.0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C52" s="2">
         <v>51.0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C53" s="2">
         <v>52.0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C54" s="2">
         <v>53.0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C55" s="2">
         <v>54.0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C56" s="2">
         <v>55.0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C57" s="2">
         <v>56.0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C58" s="2">
         <v>57.0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59">
@@ -3265,37 +3271,37 @@
         <v>12</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>14</v>
@@ -3309,25 +3315,25 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="9">
         <v>13.0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -3337,37 +3343,37 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B3" s="9">
         <v>12.0</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -3376,28 +3382,28 @@
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="9">
         <v>11.0</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -3409,87 +3415,87 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B5" s="9">
         <v>10.0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q5" s="8"/>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B6" s="9">
         <v>9.0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E6" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>406</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>405</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -3497,82 +3503,82 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q6" s="8"/>
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B7" s="9">
         <v>8.0</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="F7" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="N7" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>394</v>
-      </c>
       <c r="P7" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q7" s="8"/>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B8" s="9">
         <v>7.0</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -3583,37 +3589,37 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B9" s="9">
         <v>6.0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>391</v>
-      </c>
       <c r="H9" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -3622,22 +3628,22 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q9" s="8"/>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B10" s="9">
         <v>5.0</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -3651,22 +3657,22 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q10" s="8"/>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B11" s="9">
         <v>4.0</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -3680,25 +3686,25 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q11" s="8"/>
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" s="9">
         <v>3.0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -3711,22 +3717,22 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q12" s="8"/>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B13" s="9">
         <v>2.0</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -3740,22 +3746,22 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q13" s="8"/>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B14" s="9">
         <v>1.0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -3769,10 +3775,10 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q14" s="8"/>
     </row>
@@ -3782,22 +3788,22 @@
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -3811,11 +3817,11 @@
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -3834,20 +3840,20 @@
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -3863,11 +3869,11 @@
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -3886,11 +3892,11 @@
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -3909,11 +3915,11 @@
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -3932,11 +3938,11 @@
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -3955,11 +3961,11 @@
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -3978,11 +3984,11 @@
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -4001,11 +4007,11 @@
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -4024,11 +4030,11 @@
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -4047,11 +4053,11 @@
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -4070,11 +4076,11 @@
     </row>
     <row r="27">
       <c r="A27" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -4093,23 +4099,23 @@
     </row>
     <row r="28">
       <c r="A28" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>398</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>397</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
@@ -4124,11 +4130,11 @@
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -4147,11 +4153,11 @@
     </row>
     <row r="30">
       <c r="A30" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -4170,11 +4176,11 @@
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -4193,11 +4199,11 @@
     </row>
     <row r="32">
       <c r="A32" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -4216,11 +4222,11 @@
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -4239,11 +4245,11 @@
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -4262,11 +4268,11 @@
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -4285,11 +4291,11 @@
     </row>
     <row r="36">
       <c r="A36" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -4308,11 +4314,11 @@
     </row>
     <row r="37">
       <c r="A37" s="8" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -4331,11 +4337,11 @@
     </row>
     <row r="38">
       <c r="A38" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -4354,11 +4360,11 @@
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -4377,11 +4383,11 @@
     </row>
     <row r="40">
       <c r="A40" s="8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -4400,11 +4406,11 @@
     </row>
     <row r="41">
       <c r="A41" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -4423,11 +4429,11 @@
     </row>
     <row r="42">
       <c r="A42" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -4446,11 +4452,11 @@
     </row>
     <row r="43">
       <c r="A43" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -4469,11 +4475,11 @@
     </row>
     <row r="44">
       <c r="A44" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -4492,14 +4498,14 @@
     </row>
     <row r="45">
       <c r="A45" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
@@ -4517,11 +4523,11 @@
     </row>
     <row r="46">
       <c r="A46" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -4540,11 +4546,11 @@
     </row>
     <row r="47">
       <c r="A47" s="8" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
@@ -4563,14 +4569,14 @@
     </row>
     <row r="48">
       <c r="A48" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
@@ -4588,11 +4594,11 @@
     </row>
     <row r="49">
       <c r="A49" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -4611,11 +4617,11 @@
     </row>
     <row r="50">
       <c r="A50" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -4634,11 +4640,11 @@
     </row>
     <row r="51">
       <c r="A51" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
@@ -4657,17 +4663,17 @@
     </row>
     <row r="52">
       <c r="A52" s="8" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
@@ -4684,17 +4690,17 @@
     </row>
     <row r="53">
       <c r="A53" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
@@ -4711,11 +4717,11 @@
     </row>
     <row r="54">
       <c r="A54" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
@@ -4734,11 +4740,11 @@
     </row>
     <row r="55">
       <c r="A55" s="8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
@@ -4757,11 +4763,11 @@
     </row>
     <row r="56">
       <c r="A56" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
@@ -4780,11 +4786,11 @@
     </row>
     <row r="57">
       <c r="A57" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
@@ -4803,11 +4809,11 @@
     </row>
     <row r="58">
       <c r="A58" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
@@ -4847,31 +4853,31 @@
         <v>2</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push out new title for tanya
</commit_message>
<xml_diff>
--- a/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
+++ b/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
@@ -27,7 +27,7 @@
     <t>title</t>
   </si>
   <si>
-    <t>Change me in the spreadsheet</t>
+    <t>Oscars 2016: Every movie nominated for an Academy Award, ranked</t>
   </si>
   <si>
     <t>meta_description</t>
@@ -1331,7 +1331,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -1339,6 +1339,9 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1450,7 +1453,7 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1472,22 +1475,22 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -3261,1574 +3264,1574 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="10">
         <v>13.0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q2" s="8"/>
+      <c r="Q2" s="9"/>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="10">
         <v>12.0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q3" s="8"/>
+      <c r="Q3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="10">
         <v>11.0</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q4" s="8"/>
+      <c r="Q4" s="9"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="10">
         <v>10.0</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8" t="s">
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q5" s="8"/>
+      <c r="Q5" s="9"/>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="10">
         <v>9.0</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8" t="s">
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q6" s="8"/>
+      <c r="Q6" s="9"/>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="10">
         <v>8.0</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q7" s="8"/>
+      <c r="Q7" s="9"/>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="10">
         <v>7.0</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q8" s="8"/>
+      <c r="Q8" s="9"/>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="10">
         <v>6.0</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8" t="s">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q9" s="8"/>
+      <c r="Q9" s="9"/>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="10">
         <v>5.0</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q10" s="8"/>
+      <c r="Q10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="10">
         <v>4.0</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="P11" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q11" s="8"/>
+      <c r="Q11" s="9"/>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="10">
         <v>3.0</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P12" s="8" t="s">
+      <c r="P12" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q12" s="8"/>
+      <c r="Q12" s="9"/>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="10">
         <v>2.0</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="P13" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q13" s="8"/>
+      <c r="Q13" s="9"/>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="10">
         <v>1.0</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="P14" s="8" t="s">
+      <c r="P14" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q14" s="8"/>
+      <c r="Q14" s="9"/>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
     </row>
     <row r="16">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
     </row>
     <row r="21">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
     </row>
     <row r="22">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
     </row>
     <row r="23">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
     </row>
     <row r="24">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
     </row>
     <row r="25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
     </row>
     <row r="26">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
     </row>
     <row r="27">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
     </row>
     <row r="30">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
     </row>
     <row r="31">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
     </row>
     <row r="32">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
     </row>
     <row r="33">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8" t="s">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
     </row>
     <row r="34">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
     </row>
     <row r="35">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
     </row>
     <row r="36">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
     </row>
     <row r="37">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
     </row>
     <row r="38">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8" t="s">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
     </row>
     <row r="39">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8" t="s">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
     </row>
     <row r="40">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8" t="s">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
     </row>
     <row r="41">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8" t="s">
+      <c r="B41" s="9"/>
+      <c r="C41" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
     </row>
     <row r="42">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8" t="s">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
     </row>
     <row r="43">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8" t="s">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
     </row>
     <row r="44">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8" t="s">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
     </row>
     <row r="45">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8" t="s">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="9"/>
     </row>
     <row r="46">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8" t="s">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
     </row>
     <row r="47">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8" t="s">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
     </row>
     <row r="48">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8" t="s">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
     </row>
     <row r="49">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8" t="s">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="9"/>
     </row>
     <row r="50">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8" t="s">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
     </row>
     <row r="51">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8" t="s">
+      <c r="B51" s="9"/>
+      <c r="C51" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
     </row>
     <row r="52">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8" t="s">
+      <c r="B52" s="9"/>
+      <c r="C52" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="8"/>
-      <c r="O52" s="8"/>
-      <c r="P52" s="8"/>
-      <c r="Q52" s="8"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="9"/>
     </row>
     <row r="53">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8" t="s">
+      <c r="B53" s="9"/>
+      <c r="C53" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="8"/>
-      <c r="P53" s="8"/>
-      <c r="Q53" s="8"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
     </row>
     <row r="54">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8" t="s">
+      <c r="B54" s="9"/>
+      <c r="C54" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="8"/>
-      <c r="O54" s="8"/>
-      <c r="P54" s="8"/>
-      <c r="Q54" s="8"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="9"/>
     </row>
     <row r="55">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8" t="s">
+      <c r="B55" s="9"/>
+      <c r="C55" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="8"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="8"/>
-      <c r="O55" s="8"/>
-      <c r="P55" s="8"/>
-      <c r="Q55" s="8"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="9"/>
     </row>
     <row r="56">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8" t="s">
+      <c r="B56" s="9"/>
+      <c r="C56" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="8"/>
-      <c r="P56" s="8"/>
-      <c r="Q56" s="8"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="9"/>
     </row>
     <row r="57">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8" t="s">
+      <c r="B57" s="9"/>
+      <c r="C57" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="8"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
-      <c r="Q57" s="8"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
+      <c r="Q57" s="9"/>
     </row>
     <row r="58">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8" t="s">
+      <c r="B58" s="9"/>
+      <c r="C58" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="8"/>
-      <c r="O58" s="8"/>
-      <c r="P58" s="8"/>
-      <c r="Q58" s="8"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="9"/>
+      <c r="Q58" s="9"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -4849,34 +4852,34 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>420</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial code in place for adding oscar svg
</commit_message>
<xml_diff>
--- a/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
+++ b/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="427">
   <si>
     <t>name</t>
   </si>
@@ -87,6 +87,9 @@
     <t>availabilityFilter</t>
   </si>
   <si>
+    <t>won</t>
+  </si>
+  <si>
     <t>Carol</t>
   </si>
   <si>
@@ -112,6 +115,9 @@
   </si>
   <si>
     <t>InTheaters</t>
+  </si>
+  <si>
+    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" viewBox="0 0 40 40" class="small_logo" data-svg-fallback-override="" &gt;&lt;path fill="#FFF3C2" d="M136,315.8c-0.8-3.7-7.5-7.8-18.3-10.8c1.5-1.9,2.2-4.1,2.2-6.7c-0.2-7.2-2.2-10.7-3.9-12.3c0.2-0.5,0.3-0.9,0.3-1.4c0-5.7-13.5-10.6-31.8-12.2c0.4-2,0.4-4.1,0.4-4.1s-4.1-19.2,1.2-30.2c5.3-11,3.3-27.3,2-29.8c-1.2-2.4-2.9-14.7,0-19.6c2.8-4.9,4.1-16.3,5.7-33.9c1.6-17.6-3.3-20.8-3.3-20.8v-14.3h3.3c10.2-0.8,11.4-21.6,12.7-31c1.2-9.4,8.2-18,0-29c-8.2-11-27.3-15.1-27.3-15.1l0.4-10.2c0,0,5.3-4.5,4.9-19.6C83.2,0,70.6,0,70.6,0h-4.5c0,0-12.6,0-13.1,15.1c-0.4,15.1,4.9,19.6,4.9,19.6l0.4,10.2c0,0-19.6,4.1-27.3,15.1c-8.2,11-1.2,19.6,0,29c1.2,9.4,2.8,30.2,12.6,31h3.3v14.3c0,0-4.9,3.3-3.3,20.8c1.6,17.6,2.8,29,5.7,33.9c2.8,4.9,1.2,17.6,0,19.6c-1.2,2.4-3.3,18.8,2,29.8c5.3,11,1.2,30.2,1.2,30.2s0,1.6,0.4,4.1c-18.8,1.2-32.2,6.1-32.2,11.8c0,0.3,0.1,0.7,0.2,1c-1.8,1.6-3.8,5-4.2,12.8c0,2.6,0.7,4.9,2.2,6.7c-11.9,3.4-19,7.4-19,12.3v23.1c0,0,13.4,15.6,72.3,14.5c58.9-0.7,64.1-19,64.1-19v-20.1H136z" class="st0"&gt;&lt;/path&gt;&lt;/svg&gt;</t>
   </si>
   <si>
     <t>Mustang</t>
@@ -1548,1743 +1554,1749 @@
       <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2">
         <v>2.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2">
         <v>3.0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2">
         <v>4.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2">
         <v>5.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2">
         <v>6.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2">
         <v>7.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2">
         <v>8.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C10" s="2">
         <v>9.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C11" s="2">
         <v>10.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2">
         <v>11.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C13" s="2">
         <v>12.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C14" s="2">
         <v>13.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C15" s="2">
         <v>14.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C16" s="2">
         <v>15.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C17" s="2">
         <v>16.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C18" s="2">
         <v>17.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AA18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C19" s="2">
         <v>18.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C20" s="2">
         <v>19.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C21" s="2">
         <v>20.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C22" s="2">
         <v>21.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C23" s="2">
         <v>22.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C24" s="2">
         <v>23.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C25" s="2">
         <v>24.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C26" s="2">
         <v>25.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C27" s="2">
         <v>26.0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C28" s="2">
         <v>27.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C29" s="2">
         <v>28.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C30" s="2">
         <v>29.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C31" s="2">
         <v>30.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C32" s="2">
         <v>31.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C33" s="2">
         <v>32.0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C34" s="2">
         <v>33.0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C35" s="2">
         <v>34.0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C36" s="2">
         <v>35.0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C37" s="2">
         <v>36.0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C38" s="2">
         <v>37.0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C39" s="2">
         <v>38.0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C40" s="2">
         <v>39.0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C41" s="2">
         <v>40.0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C42" s="2">
         <v>41.0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C43" s="2">
         <v>42.0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C44" s="2">
         <v>43.0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C45" s="2">
         <v>44.0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C46" s="2">
         <v>45.0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C47" s="2">
         <v>46.0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C48" s="2">
         <v>47.0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C49" s="2">
         <v>48.0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C50" s="2">
         <v>49.0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C51" s="2">
         <v>50.0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C52" s="2">
         <v>51.0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C53" s="2">
         <v>52.0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C54" s="2">
         <v>53.0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C55" s="2">
         <v>54.0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C56" s="2">
         <v>55.0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C57" s="2">
         <v>56.0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C58" s="2">
         <v>57.0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59">
@@ -3317,37 +3329,37 @@
         <v>16</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>18</v>
@@ -3361,25 +3373,25 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="11">
         <v>13.0</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -3389,37 +3401,37 @@
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
       <c r="O2" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q2" s="10"/>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B3" s="11">
         <v>12.0</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -3428,28 +3440,28 @@
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q3" s="10"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B4" s="11">
         <v>11.0</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -3461,87 +3473,87 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B5" s="11">
         <v>10.0</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B6" s="11">
         <v>9.0</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>398</v>
-      </c>
       <c r="H6" s="10" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -3549,82 +3561,82 @@
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B7" s="11">
         <v>8.0</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B8" s="11">
         <v>7.0</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -3635,37 +3647,37 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B9" s="11">
         <v>6.0</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -3674,22 +3686,22 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B10" s="11">
         <v>5.0</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -3703,22 +3715,22 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B11" s="11">
         <v>4.0</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -3732,25 +3744,25 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B12" s="11">
         <v>3.0</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -3763,22 +3775,22 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B13" s="11">
         <v>2.0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -3792,22 +3804,22 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q13" s="10"/>
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B14" s="11">
         <v>1.0</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -3821,35 +3833,35 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q14" s="10"/>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>409</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>404</v>
-      </c>
       <c r="H15" s="10" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -3863,11 +3875,11 @@
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -3886,20 +3898,20 @@
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -3915,11 +3927,11 @@
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -3938,11 +3950,11 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -3961,11 +3973,11 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -3984,11 +3996,11 @@
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -4007,11 +4019,11 @@
     </row>
     <row r="22">
       <c r="A22" s="10" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -4030,11 +4042,11 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -4053,11 +4065,11 @@
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -4076,11 +4088,11 @@
     </row>
     <row r="25">
       <c r="A25" s="10" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -4099,11 +4111,11 @@
     </row>
     <row r="26">
       <c r="A26" s="10" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -4122,11 +4134,11 @@
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -4145,23 +4157,23 @@
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E28" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="F28" s="10" t="s">
-        <v>408</v>
-      </c>
       <c r="G28" s="10" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -4176,11 +4188,11 @@
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -4199,11 +4211,11 @@
     </row>
     <row r="30">
       <c r="A30" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -4222,11 +4234,11 @@
     </row>
     <row r="31">
       <c r="A31" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -4245,11 +4257,11 @@
     </row>
     <row r="32">
       <c r="A32" s="10" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -4268,11 +4280,11 @@
     </row>
     <row r="33">
       <c r="A33" s="10" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="10" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -4291,11 +4303,11 @@
     </row>
     <row r="34">
       <c r="A34" s="10" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -4314,11 +4326,11 @@
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -4337,11 +4349,11 @@
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -4360,11 +4372,11 @@
     </row>
     <row r="37">
       <c r="A37" s="10" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
@@ -4383,11 +4395,11 @@
     </row>
     <row r="38">
       <c r="A38" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
@@ -4406,11 +4418,11 @@
     </row>
     <row r="39">
       <c r="A39" s="10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -4429,11 +4441,11 @@
     </row>
     <row r="40">
       <c r="A40" s="10" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -4452,11 +4464,11 @@
     </row>
     <row r="41">
       <c r="A41" s="10" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -4475,11 +4487,11 @@
     </row>
     <row r="42">
       <c r="A42" s="10" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -4498,11 +4510,11 @@
     </row>
     <row r="43">
       <c r="A43" s="10" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -4521,11 +4533,11 @@
     </row>
     <row r="44">
       <c r="A44" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="10" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -4544,14 +4556,14 @@
     </row>
     <row r="45">
       <c r="A45" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -4569,11 +4581,11 @@
     </row>
     <row r="46">
       <c r="A46" s="10" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
@@ -4592,11 +4604,11 @@
     </row>
     <row r="47">
       <c r="A47" s="10" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
@@ -4615,14 +4627,14 @@
     </row>
     <row r="48">
       <c r="A48" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -4640,11 +4652,11 @@
     </row>
     <row r="49">
       <c r="A49" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
@@ -4663,11 +4675,11 @@
     </row>
     <row r="50">
       <c r="A50" s="10" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
@@ -4686,11 +4698,11 @@
     </row>
     <row r="51">
       <c r="A51" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
@@ -4709,17 +4721,17 @@
     </row>
     <row r="52">
       <c r="A52" s="10" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
@@ -4736,17 +4748,17 @@
     </row>
     <row r="53">
       <c r="A53" s="10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="10" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
@@ -4763,11 +4775,11 @@
     </row>
     <row r="54">
       <c r="A54" s="10" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
@@ -4786,11 +4798,11 @@
     </row>
     <row r="55">
       <c r="A55" s="10" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
@@ -4809,11 +4821,11 @@
     </row>
     <row r="56">
       <c r="A56" s="10" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
@@ -4832,11 +4844,11 @@
     </row>
     <row r="57">
       <c r="A57" s="10" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
@@ -4855,11 +4867,11 @@
     </row>
     <row r="58">
       <c r="A58" s="10" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
@@ -4899,31 +4911,31 @@
         <v>2</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="14" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost in place for 5 or more winners
</commit_message>
<xml_diff>
--- a/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
+++ b/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="438">
   <si>
     <t>name</t>
   </si>
@@ -87,7 +87,40 @@
     <t>availabilityFilter</t>
   </si>
   <si>
-    <t>won</t>
+    <t>wonOne</t>
+  </si>
+  <si>
+    <t>wonTwo</t>
+  </si>
+  <si>
+    <t>wonThree</t>
+  </si>
+  <si>
+    <t>wonFour</t>
+  </si>
+  <si>
+    <t>wonFive</t>
+  </si>
+  <si>
+    <t>wonSix</t>
+  </si>
+  <si>
+    <t>wonSeven</t>
+  </si>
+  <si>
+    <t>wonEight</t>
+  </si>
+  <si>
+    <t>wonNine</t>
+  </si>
+  <si>
+    <t>wonTen</t>
+  </si>
+  <si>
+    <t>wonEleven</t>
+  </si>
+  <si>
+    <t>wonTwelve</t>
   </si>
   <si>
     <t>Carol</t>
@@ -117,7 +150,7 @@
     <t>InTheaters</t>
   </si>
   <si>
-    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" viewBox="0 0 40 40" class="small_logo" data-svg-fallback-override="" &gt;&lt;path fill="#FFF3C2" d="M136,315.8c-0.8-3.7-7.5-7.8-18.3-10.8c1.5-1.9,2.2-4.1,2.2-6.7c-0.2-7.2-2.2-10.7-3.9-12.3c0.2-0.5,0.3-0.9,0.3-1.4c0-5.7-13.5-10.6-31.8-12.2c0.4-2,0.4-4.1,0.4-4.1s-4.1-19.2,1.2-30.2c5.3-11,3.3-27.3,2-29.8c-1.2-2.4-2.9-14.7,0-19.6c2.8-4.9,4.1-16.3,5.7-33.9c1.6-17.6-3.3-20.8-3.3-20.8v-14.3h3.3c10.2-0.8,11.4-21.6,12.7-31c1.2-9.4,8.2-18,0-29c-8.2-11-27.3-15.1-27.3-15.1l0.4-10.2c0,0,5.3-4.5,4.9-19.6C83.2,0,70.6,0,70.6,0h-4.5c0,0-12.6,0-13.1,15.1c-0.4,15.1,4.9,19.6,4.9,19.6l0.4,10.2c0,0-19.6,4.1-27.3,15.1c-8.2,11-1.2,19.6,0,29c1.2,9.4,2.8,30.2,12.6,31h3.3v14.3c0,0-4.9,3.3-3.3,20.8c1.6,17.6,2.8,29,5.7,33.9c2.8,4.9,1.2,17.6,0,19.6c-1.2,2.4-3.3,18.8,2,29.8c5.3,11,1.2,30.2,1.2,30.2s0,1.6,0.4,4.1c-18.8,1.2-32.2,6.1-32.2,11.8c0,0.3,0.1,0.7,0.2,1c-1.8,1.6-3.8,5-4.2,12.8c0,2.6,0.7,4.9,2.2,6.7c-11.9,3.4-19,7.4-19,12.3v23.1c0,0,13.4,15.6,72.3,14.5c58.9-0.7,64.1-19,64.1-19v-20.1H136z" class="st0"&gt;&lt;/path&gt;&lt;/svg&gt;</t>
+    <t>y</t>
   </si>
   <si>
     <t>Mustang</t>
@@ -1557,1746 +1590,1818 @@
       <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2">
         <v>2.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2">
         <v>3.0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="O4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2">
         <v>4.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2">
         <v>5.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C7" s="2">
         <v>6.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2">
         <v>7.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C9" s="2">
         <v>8.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C10" s="2">
         <v>9.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C11" s="2">
         <v>10.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>88</v>
+      <c r="T11" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C12" s="2">
         <v>11.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="C13" s="2">
         <v>12.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="J13" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C14" s="2">
         <v>13.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C15" s="2">
         <v>14.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C16" s="2">
         <v>15.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C17" s="2">
         <v>16.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="C18" s="2">
         <v>17.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="AA18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C19" s="2">
         <v>18.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="C20" s="2">
         <v>19.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="C21" s="2">
         <v>20.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C22" s="2">
         <v>21.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="C23" s="2">
         <v>22.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C24" s="2">
         <v>23.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="C25" s="2">
         <v>24.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="C26" s="2">
         <v>25.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="C27" s="2">
         <v>26.0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="C28" s="2">
         <v>27.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="C29" s="2">
         <v>28.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="C30" s="2">
         <v>29.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C31" s="2">
         <v>30.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="C32" s="2">
         <v>31.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="C33" s="2">
         <v>32.0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="C34" s="2">
         <v>33.0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="C35" s="2">
         <v>34.0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="C36" s="2">
         <v>35.0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="C37" s="2">
         <v>36.0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="C38" s="2">
         <v>37.0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="C39" s="2">
         <v>38.0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="C40" s="2">
         <v>39.0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="C41" s="2">
         <v>40.0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="C42" s="2">
         <v>41.0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="C43" s="2">
         <v>42.0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="C44" s="2">
         <v>43.0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="C45" s="2">
         <v>44.0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="C46" s="2">
         <v>45.0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="C47" s="2">
         <v>46.0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="C48" s="2">
         <v>47.0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="C49" s="2">
         <v>48.0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>326</v>
+        <v>337</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="C50" s="2">
         <v>49.0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="C51" s="2">
         <v>50.0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="C52" s="2">
         <v>51.0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
       <c r="C53" s="2">
         <v>52.0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="C54" s="2">
         <v>53.0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
       <c r="C55" s="2">
         <v>54.0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="C56" s="2">
         <v>55.0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="C57" s="2">
         <v>56.0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="C58" s="2">
         <v>57.0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59">
@@ -3329,37 +3434,37 @@
         <v>16</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>395</v>
+        <v>406</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>18</v>
@@ -3373,25 +3478,25 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B2" s="11">
         <v>13.0</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -3401,37 +3506,37 @@
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
       <c r="O2" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q2" s="10"/>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B3" s="11">
         <v>12.0</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -3440,28 +3545,28 @@
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q3" s="10"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B4" s="11">
         <v>11.0</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -3473,87 +3578,87 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="B5" s="11">
         <v>10.0</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>397</v>
-      </c>
       <c r="F5" s="10" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>412</v>
+        <v>423</v>
       </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="B6" s="11">
         <v>9.0</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>412</v>
+        <v>423</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -3561,82 +3666,82 @@
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="B7" s="11">
         <v>8.0</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>397</v>
-      </c>
       <c r="F7" s="10" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="G7" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>405</v>
-      </c>
-      <c r="L7" s="10" t="s">
+      <c r="O7" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>401</v>
-      </c>
       <c r="P7" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B8" s="11">
         <v>7.0</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -3647,37 +3752,37 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B9" s="11">
         <v>6.0</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -3686,22 +3791,22 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B10" s="11">
         <v>5.0</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -3715,22 +3820,22 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
       <c r="B11" s="11">
         <v>4.0</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -3744,25 +3849,25 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B12" s="11">
         <v>3.0</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -3775,22 +3880,22 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B13" s="11">
         <v>2.0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -3804,22 +3909,22 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q13" s="10"/>
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B14" s="11">
         <v>1.0</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -3833,35 +3938,35 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q14" s="10"/>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -3875,11 +3980,11 @@
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -3898,20 +4003,20 @@
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -3927,11 +4032,11 @@
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -3950,11 +4055,11 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -3973,11 +4078,11 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -3996,11 +4101,11 @@
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -4019,11 +4124,11 @@
     </row>
     <row r="22">
       <c r="A22" s="10" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -4042,11 +4147,11 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -4065,11 +4170,11 @@
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -4088,11 +4193,11 @@
     </row>
     <row r="25">
       <c r="A25" s="10" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -4111,11 +4216,11 @@
     </row>
     <row r="26">
       <c r="A26" s="10" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -4134,11 +4239,11 @@
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -4157,23 +4262,23 @@
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>412</v>
+        <v>423</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -4188,11 +4293,11 @@
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -4211,11 +4316,11 @@
     </row>
     <row r="30">
       <c r="A30" s="10" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -4234,11 +4339,11 @@
     </row>
     <row r="31">
       <c r="A31" s="10" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -4257,11 +4362,11 @@
     </row>
     <row r="32">
       <c r="A32" s="10" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -4280,11 +4385,11 @@
     </row>
     <row r="33">
       <c r="A33" s="10" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="10" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -4303,11 +4408,11 @@
     </row>
     <row r="34">
       <c r="A34" s="10" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -4326,11 +4431,11 @@
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -4349,11 +4454,11 @@
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -4372,11 +4477,11 @@
     </row>
     <row r="37">
       <c r="A37" s="10" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
@@ -4395,11 +4500,11 @@
     </row>
     <row r="38">
       <c r="A38" s="10" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
@@ -4418,11 +4523,11 @@
     </row>
     <row r="39">
       <c r="A39" s="10" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -4441,11 +4546,11 @@
     </row>
     <row r="40">
       <c r="A40" s="10" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -4464,11 +4569,11 @@
     </row>
     <row r="41">
       <c r="A41" s="10" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -4487,11 +4592,11 @@
     </row>
     <row r="42">
       <c r="A42" s="10" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -4510,11 +4615,11 @@
     </row>
     <row r="43">
       <c r="A43" s="10" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -4533,11 +4638,11 @@
     </row>
     <row r="44">
       <c r="A44" s="10" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="10" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -4556,14 +4661,14 @@
     </row>
     <row r="45">
       <c r="A45" s="10" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -4581,11 +4686,11 @@
     </row>
     <row r="46">
       <c r="A46" s="10" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
@@ -4604,11 +4709,11 @@
     </row>
     <row r="47">
       <c r="A47" s="10" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
@@ -4627,14 +4732,14 @@
     </row>
     <row r="48">
       <c r="A48" s="10" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -4652,11 +4757,11 @@
     </row>
     <row r="49">
       <c r="A49" s="10" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
@@ -4675,11 +4780,11 @@
     </row>
     <row r="50">
       <c r="A50" s="10" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
@@ -4698,11 +4803,11 @@
     </row>
     <row r="51">
       <c r="A51" s="10" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
@@ -4721,17 +4826,17 @@
     </row>
     <row r="52">
       <c r="A52" s="10" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
@@ -4748,17 +4853,17 @@
     </row>
     <row r="53">
       <c r="A53" s="10" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="10" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>412</v>
+        <v>423</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
@@ -4775,11 +4880,11 @@
     </row>
     <row r="54">
       <c r="A54" s="10" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
@@ -4798,11 +4903,11 @@
     </row>
     <row r="55">
       <c r="A55" s="10" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
@@ -4821,11 +4926,11 @@
     </row>
     <row r="56">
       <c r="A56" s="10" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
@@ -4844,11 +4949,11 @@
     </row>
     <row r="57">
       <c r="A57" s="10" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
@@ -4867,11 +4972,11 @@
     </row>
     <row r="58">
       <c r="A58" s="10" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
@@ -4911,31 +5016,31 @@
         <v>2</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="14" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
styles in place for oscar winners
</commit_message>
<xml_diff>
--- a/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
+++ b/google_drive_cache/1nH4LH15wO3nx31vO9CtqP3HkJItg98LdxMHsy321TQw.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="426">
   <si>
     <t>name</t>
   </si>
@@ -87,40 +87,7 @@
     <t>availabilityFilter</t>
   </si>
   <si>
-    <t>wonOne</t>
-  </si>
-  <si>
-    <t>wonTwo</t>
-  </si>
-  <si>
-    <t>wonThree</t>
-  </si>
-  <si>
-    <t>wonFour</t>
-  </si>
-  <si>
-    <t>wonFive</t>
-  </si>
-  <si>
-    <t>wonSix</t>
-  </si>
-  <si>
-    <t>wonSeven</t>
-  </si>
-  <si>
-    <t>wonEight</t>
-  </si>
-  <si>
-    <t>wonNine</t>
-  </si>
-  <si>
-    <t>wonTen</t>
-  </si>
-  <si>
-    <t>wonEleven</t>
-  </si>
-  <si>
-    <t>wonTwelve</t>
+    <t>won</t>
   </si>
   <si>
     <t>Carol</t>
@@ -148,9 +115,6 @@
   </si>
   <si>
     <t>InTheaters</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
   <si>
     <t>Mustang</t>
@@ -1590,1818 +1554,1785 @@
       <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="K2" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2">
         <v>2.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="K3" s="2">
+        <v>6.0</v>
       </c>
       <c r="N3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2">
         <v>3.0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="K4" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="M4" s="2"/>
       <c r="O4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2">
         <v>4.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="K5" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="N5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2">
         <v>5.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="O6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2">
         <v>6.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="P7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C8" s="2">
         <v>7.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="Q8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2">
         <v>8.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="R9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C10" s="2">
         <v>9.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="S10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2">
         <v>10.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="T11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C12" s="2">
         <v>11.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="U12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C13" s="2">
         <v>12.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="V13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2">
         <v>13.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C15" s="2">
         <v>14.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C16" s="2">
         <v>15.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C17" s="2">
         <v>16.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C18" s="2">
         <v>17.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="AA18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C19" s="2">
         <v>18.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C20" s="2">
         <v>19.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C21" s="2">
         <v>20.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C22" s="2">
         <v>21.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C23" s="2">
         <v>22.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C24" s="2">
         <v>23.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C25" s="2">
         <v>24.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C26" s="2">
         <v>25.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C27" s="2">
         <v>26.0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C28" s="2">
         <v>27.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C29" s="2">
         <v>28.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="C30" s="2">
         <v>29.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C31" s="2">
         <v>30.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="C32" s="2">
         <v>31.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C33" s="2">
         <v>32.0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="C34" s="2">
         <v>33.0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C35" s="2">
         <v>34.0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C36" s="2">
         <v>35.0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="C37" s="2">
         <v>36.0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="C38" s="2">
         <v>37.0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="C39" s="2">
         <v>38.0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C40" s="2">
         <v>39.0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C41" s="2">
         <v>40.0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="C42" s="2">
         <v>41.0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C43" s="2">
         <v>42.0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="C44" s="2">
         <v>43.0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="C45" s="2">
         <v>44.0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="C46" s="2">
         <v>45.0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C47" s="2">
         <v>46.0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="C48" s="2">
         <v>47.0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="C49" s="2">
         <v>48.0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="C50" s="2">
         <v>49.0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="C51" s="2">
         <v>50.0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="C52" s="2">
         <v>51.0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="C53" s="2">
         <v>52.0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="C54" s="2">
         <v>53.0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="C55" s="2">
         <v>54.0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="C56" s="2">
         <v>55.0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="C57" s="2">
         <v>56.0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="C58" s="2">
         <v>57.0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59">
@@ -3434,37 +3365,37 @@
         <v>16</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>18</v>
@@ -3478,25 +3409,25 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B2" s="11">
         <v>13.0</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -3506,37 +3437,37 @@
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
       <c r="O2" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q2" s="10"/>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B3" s="11">
         <v>12.0</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -3545,28 +3476,28 @@
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q3" s="10"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B4" s="11">
         <v>11.0</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -3578,87 +3509,87 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="B5" s="11">
         <v>10.0</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>419</v>
-      </c>
       <c r="E5" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="H5" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>422</v>
-      </c>
       <c r="K5" s="10" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="B6" s="11">
         <v>9.0</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>411</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>423</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -3666,82 +3597,82 @@
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="B7" s="11">
         <v>8.0</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>419</v>
-      </c>
       <c r="E7" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="H7" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>422</v>
-      </c>
       <c r="K7" s="10" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B8" s="11">
         <v>7.0</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -3752,37 +3683,37 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B9" s="11">
         <v>6.0</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -3791,22 +3722,22 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B10" s="11">
         <v>5.0</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -3820,22 +3751,22 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="B11" s="11">
         <v>4.0</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -3849,25 +3780,25 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B12" s="11">
         <v>3.0</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -3880,22 +3811,22 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B13" s="11">
         <v>2.0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -3909,22 +3840,22 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q13" s="10"/>
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B14" s="11">
         <v>1.0</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -3938,35 +3869,35 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="Q14" s="10"/>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -3980,11 +3911,11 @@
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -4003,20 +3934,20 @@
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>413</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>425</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -4032,11 +3963,11 @@
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -4055,11 +3986,11 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -4078,11 +4009,11 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -4101,11 +4032,11 @@
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -4124,11 +4055,11 @@
     </row>
     <row r="22">
       <c r="A22" s="10" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -4147,11 +4078,11 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -4170,11 +4101,11 @@
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -4193,11 +4124,11 @@
     </row>
     <row r="25">
       <c r="A25" s="10" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -4216,11 +4147,11 @@
     </row>
     <row r="26">
       <c r="A26" s="10" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -4239,11 +4170,11 @@
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -4262,23 +4193,23 @@
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -4293,11 +4224,11 @@
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -4316,11 +4247,11 @@
     </row>
     <row r="30">
       <c r="A30" s="10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -4339,11 +4270,11 @@
     </row>
     <row r="31">
       <c r="A31" s="10" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -4362,11 +4293,11 @@
     </row>
     <row r="32">
       <c r="A32" s="10" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -4385,11 +4316,11 @@
     </row>
     <row r="33">
       <c r="A33" s="10" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="10" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -4408,11 +4339,11 @@
     </row>
     <row r="34">
       <c r="A34" s="10" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -4431,11 +4362,11 @@
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -4454,11 +4385,11 @@
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -4477,11 +4408,11 @@
     </row>
     <row r="37">
       <c r="A37" s="10" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
@@ -4500,11 +4431,11 @@
     </row>
     <row r="38">
       <c r="A38" s="10" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
@@ -4523,11 +4454,11 @@
     </row>
     <row r="39">
       <c r="A39" s="10" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -4546,11 +4477,11 @@
     </row>
     <row r="40">
       <c r="A40" s="10" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -4569,11 +4500,11 @@
     </row>
     <row r="41">
       <c r="A41" s="10" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -4592,11 +4523,11 @@
     </row>
     <row r="42">
       <c r="A42" s="10" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -4615,11 +4546,11 @@
     </row>
     <row r="43">
       <c r="A43" s="10" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -4638,11 +4569,11 @@
     </row>
     <row r="44">
       <c r="A44" s="10" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="10" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -4661,14 +4592,14 @@
     </row>
     <row r="45">
       <c r="A45" s="10" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="D45" s="10" t="s">
         <v>421</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>433</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -4686,11 +4617,11 @@
     </row>
     <row r="46">
       <c r="A46" s="10" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
@@ -4709,11 +4640,11 @@
     </row>
     <row r="47">
       <c r="A47" s="10" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
@@ -4732,14 +4663,14 @@
     </row>
     <row r="48">
       <c r="A48" s="10" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -4757,11 +4688,11 @@
     </row>
     <row r="49">
       <c r="A49" s="10" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
@@ -4780,11 +4711,11 @@
     </row>
     <row r="50">
       <c r="A50" s="10" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
@@ -4803,11 +4734,11 @@
     </row>
     <row r="51">
       <c r="A51" s="10" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
@@ -4826,17 +4757,17 @@
     </row>
     <row r="52">
       <c r="A52" s="10" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
@@ -4853,17 +4784,17 @@
     </row>
     <row r="53">
       <c r="A53" s="10" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="10" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
@@ -4880,11 +4811,11 @@
     </row>
     <row r="54">
       <c r="A54" s="10" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
@@ -4903,11 +4834,11 @@
     </row>
     <row r="55">
       <c r="A55" s="10" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
@@ -4926,11 +4857,11 @@
     </row>
     <row r="56">
       <c r="A56" s="10" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
@@ -4949,11 +4880,11 @@
     </row>
     <row r="57">
       <c r="A57" s="10" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
@@ -4972,11 +4903,11 @@
     </row>
     <row r="58">
       <c r="A58" s="10" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
@@ -5016,31 +4947,31 @@
         <v>2</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="14" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>